<commit_message>
More tests for excel_to_html.
</commit_message>
<xml_diff>
--- a/tests/test_excel_to_html/test_normal_unmerged.xlsx
+++ b/tests/test_excel_to_html/test_normal_unmerged.xlsx
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -127,12 +128,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>